<commit_message>
Finishing touches before Toby Carpentries Meeting
</commit_message>
<xml_diff>
--- a/sample_toastui_excel.xlsx
+++ b/sample_toastui_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jqiu/Documents/CBWgithub/cbw-dev-test-pages/INR-2024-Recreate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7617B9BD-BC95-804B-B56C-04149ECE5430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F32ABA-AF68-0245-AE8C-CCDBF86B2F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30340" yWindow="-23080" windowWidth="28040" windowHeight="17240" xr2:uid="{4BF95482-EF90-AE42-B200-12889CD43DD1}"/>
+    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17240" xr2:uid="{4BF95482-EF90-AE42-B200-12889CD43DD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -457,7 +457,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>